<commit_message>
2023 demand data collection
Also, weekend 6PM-10PM data collection for the year 2023
</commit_message>
<xml_diff>
--- a/DeseasonalizedWeekendsF1.xlsx
+++ b/DeseasonalizedWeekendsF1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Documents\GitHub\earth-hour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF5EE57-D366-43A0-970B-34D154E3B62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A4C046-E8BC-47F2-8AF4-E9CA4A7E4B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="210">
   <si>
     <t>07Jan-08Jan</t>
   </si>
@@ -2327,7 +2327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F565B212-A568-4F9B-B951-FB958E0A2638}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2769,12 +2769,436 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF704FA-7A57-4B3E-98F8-096A7444149C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>110768.79309203901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>110180.35862964259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>101037.35365170331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>102569.8714283099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>103652.5880219853</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>105489.6587806874</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>106550.2612862548</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>106770.0676989444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>99242.402498299518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>102989.79566850699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>105266.8702056771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>104277.88173043181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>104507.391589005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>103803.36416431741</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>107893.21880058511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>107728.7567571343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>105305.68813733679</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>106528.2878560813</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>109206.86660674569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>105244.1554141605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>106359.6940331059</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>103005.6602175969</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>107532.9148656321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>105510.38955361499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>105215.4267140382</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>104423.1932100478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>105101.22683635241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>103729.8596960111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>103859.0053991366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>104595.9628707378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>106574.5571561523</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>105928.4054998764</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>103480.7593371425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>105079.972774037</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>105374.3734722899</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>102849.0898070931</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>106943.42025951399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>103575.89899272579</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>103298.5258705218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>110182.02171206981</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>109447.7106363498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>104720.05875072371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>105939.3168219752</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>107924.8897817336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>105906.7896748292</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>106847.73781658171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>104565.6777242027</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>105411.2916825182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>108067.3287371935</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>106068.00830065169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>104430.11714667649</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>103861.7363291918</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>